<commit_message>
commited by Basu 02052019
</commit_message>
<xml_diff>
--- a/upload/File/ProductsUploadTemplate.xlsx
+++ b/upload/File/ProductsUploadTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="204" yWindow="516" windowWidth="22716" windowHeight="8940"/>
+    <workbookView xWindow="210" yWindow="510" windowWidth="19440" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Product Details" sheetId="1" r:id="rId1"/>
@@ -374,17 +374,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
commited by basu 03052019
</commit_message>
<xml_diff>
--- a/upload/File/ProductsUploadTemplate.xlsx
+++ b/upload/File/ProductsUploadTemplate.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="510" windowWidth="19440" windowHeight="8940"/>
+    <workbookView xWindow="240" yWindow="540" windowWidth="18855" windowHeight="11190"/>
   </bookViews>
   <sheets>
     <sheet name="Product Details" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Category</t>
   </si>
@@ -25,20 +25,109 @@
     <t>Product Name</t>
   </si>
   <si>
+    <t>Product Description</t>
+  </si>
+  <si>
+    <t>Stock Limit</t>
+  </si>
+  <si>
+    <t>Pack Date(dd-mm-yyyy)</t>
+  </si>
+  <si>
+    <t>Exp Date(dd-mm-yyyy)</t>
+  </si>
+  <si>
+    <t>UOM</t>
+  </si>
+  <si>
+    <t>MRP</t>
+  </si>
+  <si>
+    <t>Pur Rate</t>
+  </si>
+  <si>
+    <t>Sale Rate</t>
+  </si>
+  <si>
+    <t>Tax %</t>
+  </si>
+  <si>
+    <t>Stock Qty</t>
+  </si>
+  <si>
+    <t>Online Qty</t>
+  </si>
+  <si>
+    <t>Offline Qty</t>
+  </si>
+  <si>
     <t>Vegetables</t>
   </si>
   <si>
     <t>sub category 1</t>
   </si>
   <si>
-    <t>Tomato</t>
+    <t>Brinjal</t>
+  </si>
+  <si>
+    <t>Brinjal is a very beautiful vegetable.
+it dark purple in colour.In northern sides people eat baingan ka bharta which is very tasty.brinjal is mostly grown in India and sri Lanka.brinjal is very good for health.
+brinjal is very tasty.</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>broccoli</t>
+  </si>
+  <si>
+    <t>Broccoli is popular and widely eaten. It has a distinctive ‘mustardy’ taste and well known health benefits. The stalks, buds and most of the leaves of broccoli are edible.</t>
+  </si>
+  <si>
+    <t>Puha</t>
+  </si>
+  <si>
+    <t>Traditionally it was one of the staple green vegetables of the Maori and is still eaten today. Puha can be found growing wild. The smooth leaved puha is the most popular, however, the slightly bitter and prickly leaved puha is also eaten.</t>
+  </si>
+  <si>
+    <t>sub category 2</t>
+  </si>
+  <si>
+    <t>Bundle</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Pc/Pack In Box</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -48,6 +137,19 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,10 +172,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -371,20 +506,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:16" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -394,28 +543,175 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="18" customHeight="1">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+    <row r="2" spans="1:16" ht="105">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="11">
+        <v>22</v>
+      </c>
+      <c r="J2" s="11">
+        <v>20</v>
+      </c>
+      <c r="K2" s="11">
+        <v>22</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" customHeight="1">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
+    <row r="3" spans="1:16" ht="75">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="11">
+        <v>20</v>
+      </c>
+      <c r="J3" s="11">
+        <v>18</v>
+      </c>
+      <c r="K3" s="11">
+        <v>20</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="105">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="11">
+        <v>10</v>
+      </c>
+      <c r="J4" s="11">
+        <v>8</v>
+      </c>
+      <c r="K4" s="11">
+        <v>10</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>